<commit_message>
teams daily & weekly, log
</commit_message>
<xml_diff>
--- a/public/import/weekly_template.xlsx
+++ b/public/import/weekly_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-A4\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>year</t>
   </si>
@@ -36,50 +36,27 @@
     <t>value_plan_result</t>
   </si>
   <si>
+    <t>contoh task weekly non</t>
+  </si>
+  <si>
     <t>NON</t>
   </si>
   <si>
-    <t>Audit Mutasi Bank Harian.</t>
-  </si>
-  <si>
-    <t>Audit Pembelian.</t>
-  </si>
-  <si>
-    <t>Audit Laporan Keuangan.</t>
-  </si>
-  <si>
-    <t>Audit Retur Supplier.</t>
-  </si>
-  <si>
-    <t>Audit Kas Besar Cirebon.</t>
-  </si>
-  <si>
-    <t>Audit Biaya.</t>
-  </si>
-  <si>
-    <t>Audit AR.</t>
-  </si>
-  <si>
-    <t>Pengiriman rencana kerja &amp; realisasi todolist tepat waktu.</t>
+    <t>contoh task weekly result</t>
+  </si>
+  <si>
+    <t>RESULT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,10 +79,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,150 +385,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B2" s="2">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2">
+        <v>2023</v>
+      </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B3" s="2">
-        <v>35</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3">
+        <v>2023</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B4" s="2">
-        <v>35</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B5" s="2">
-        <v>35</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B6" s="2">
-        <v>35</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B7" s="2">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B8" s="2">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B9" s="2">
-        <v>35</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2"/>
+      <c r="E3">
+        <v>10000</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>